<commit_message>
adding host col data to test metadata file
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482940D7-A82A-1444-8BF2-76F465ED8CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBFDD53-EA44-BB45-9D60-6A538A292B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="429">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4146,6 +4146,9 @@
   </si>
   <si>
     <t>OH0002.fasta</t>
+  </si>
+  <si>
+    <t>human</t>
   </si>
 </sst>
 </file>
@@ -4918,9 +4921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4958,7 +4961,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5064,7 +5067,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5206,7 +5209,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5280,7 +5283,7 @@
   <dimension ref="A1:AL46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5452,6 +5455,9 @@
       <c r="E3" t="s">
         <v>377</v>
       </c>
+      <c r="G3" t="s">
+        <v>428</v>
+      </c>
       <c r="H3" t="s">
         <v>386</v>
       </c>
@@ -5519,6 +5525,9 @@
       <c r="E4" t="s">
         <v>378</v>
       </c>
+      <c r="G4" t="s">
+        <v>428</v>
+      </c>
       <c r="H4" t="s">
         <v>386</v>
       </c>
@@ -5583,6 +5592,9 @@
       <c r="E5" t="s">
         <v>379</v>
       </c>
+      <c r="G5" t="s">
+        <v>428</v>
+      </c>
       <c r="H5" t="s">
         <v>386</v>
       </c>
@@ -5647,6 +5659,9 @@
       <c r="E6" t="s">
         <v>380</v>
       </c>
+      <c r="G6" t="s">
+        <v>428</v>
+      </c>
       <c r="H6" t="s">
         <v>386</v>
       </c>
@@ -5714,6 +5729,9 @@
       <c r="E7" t="s">
         <v>381</v>
       </c>
+      <c r="G7" t="s">
+        <v>428</v>
+      </c>
       <c r="H7" t="s">
         <v>386</v>
       </c>
@@ -5781,6 +5799,9 @@
       <c r="E8" t="s">
         <v>381</v>
       </c>
+      <c r="G8" t="s">
+        <v>428</v>
+      </c>
       <c r="H8" t="s">
         <v>386</v>
       </c>
@@ -5847,6 +5868,9 @@
       </c>
       <c r="E9" t="s">
         <v>381</v>
+      </c>
+      <c r="G9" t="s">
+        <v>428</v>
       </c>
       <c r="H9" t="s">
         <v>386</v>
@@ -9997,12 +10021,51 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -10015,51 +10078,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated submission subworkflow to full and sra
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBFDD53-EA44-BB45-9D60-6A538A292B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9195130-6292-BA40-A463-EE2266FC9555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,6 +42,20 @@
     <author>Weigand, Michael Richard (CDC/DDID/NCIRD/DBD)</author>
   </authors>
   <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{57D25698-B1C8-B144-846F-562211A73B19}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Sample identifier that matches internal fasta header name: eg 'FL001'
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{EF23935C-B24C-4C79-8489-6820FB597F4D}">
       <text>
         <r>
@@ -4124,9 +4138,6 @@
     <t>host</t>
   </si>
   <si>
-    <t>fasta_file_name</t>
-  </si>
-  <si>
     <t>FL0004.fasta</t>
   </si>
   <si>
@@ -4149,6 +4160,9 @@
   </si>
   <si>
     <t>human</t>
+  </si>
+  <si>
+    <t>fasta_name</t>
   </si>
 </sst>
 </file>
@@ -4921,9 +4935,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4961,7 +4975,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5067,7 +5081,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5209,7 +5223,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5283,49 +5297,48 @@
   <dimension ref="A1:AL46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="23.5" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" customWidth="1"/>
-    <col min="23" max="23" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>321</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>322</v>
       </c>
+      <c r="V1" s="28" t="s">
+        <v>325</v>
+      </c>
       <c r="W1" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="X1" s="28" t="s">
         <v>323</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>413</v>
@@ -5441,7 +5454,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B3" t="s">
         <v>372</v>
@@ -5456,7 +5469,7 @@
         <v>377</v>
       </c>
       <c r="G3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H3" t="s">
         <v>386</v>
@@ -5511,7 +5524,7 @@
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B4" t="s">
         <v>373</v>
@@ -5526,7 +5539,7 @@
         <v>378</v>
       </c>
       <c r="G4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H4" t="s">
         <v>386</v>
@@ -5578,7 +5591,7 @@
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B5" t="s">
         <v>374</v>
@@ -5593,7 +5606,7 @@
         <v>379</v>
       </c>
       <c r="G5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H5" t="s">
         <v>386</v>
@@ -5645,7 +5658,7 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B6" t="s">
         <v>375</v>
@@ -5660,7 +5673,7 @@
         <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H6" t="s">
         <v>386</v>
@@ -5715,7 +5728,7 @@
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B7" t="s">
         <v>376</v>
@@ -5730,7 +5743,7 @@
         <v>381</v>
       </c>
       <c r="G7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H7" t="s">
         <v>386</v>
@@ -5785,7 +5798,7 @@
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B8" t="s">
         <v>411</v>
@@ -5800,7 +5813,7 @@
         <v>381</v>
       </c>
       <c r="G8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H8" t="s">
         <v>386</v>
@@ -5855,7 +5868,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B9" t="s">
         <v>412</v>
@@ -5870,7 +5883,7 @@
         <v>381</v>
       </c>
       <c r="G9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H9" t="s">
         <v>386</v>
@@ -5924,305 +5937,305 @@
       <c r="AF9" s="28"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E10" s="28"/>
-      <c r="P10" s="28"/>
-      <c r="T10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="V10" s="28"/>
       <c r="W10" s="28"/>
-      <c r="X10" s="28"/>
-      <c r="AF10" s="28"/>
+      <c r="AE10" s="28"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="T11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="V11" s="28"/>
       <c r="W11" s="28"/>
-      <c r="X11" s="28"/>
-      <c r="AF11" s="28"/>
+      <c r="AE11" s="28"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="T12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="V12" s="28"/>
       <c r="W12" s="28"/>
-      <c r="X12" s="28"/>
-      <c r="AF12" s="28"/>
+      <c r="AE12" s="28"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="T13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="AF13" s="28"/>
+      <c r="AE13" s="28"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="T14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="V14" s="28"/>
       <c r="W14" s="28"/>
-      <c r="X14" s="28"/>
-      <c r="AF14" s="28"/>
+      <c r="AE14" s="28"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="T15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="O15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="V15" s="28"/>
       <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="AF15" s="28"/>
+      <c r="AE15" s="28"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="E16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="T16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="V16" s="28"/>
       <c r="W16" s="28"/>
-      <c r="X16" s="28"/>
-      <c r="AF16" s="28"/>
-    </row>
-    <row r="17" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="T17" s="28"/>
+      <c r="AE16" s="28"/>
+    </row>
+    <row r="17" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="V17" s="28"/>
       <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="AF17" s="28"/>
-    </row>
-    <row r="18" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="T18" s="28"/>
+      <c r="AE17" s="28"/>
+    </row>
+    <row r="18" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="V18" s="28"/>
       <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="AF18" s="28"/>
-    </row>
-    <row r="19" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E19" s="28"/>
-      <c r="P19" s="28"/>
-      <c r="T19" s="28"/>
+      <c r="AE18" s="28"/>
+    </row>
+    <row r="19" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="V19" s="28"/>
       <c r="W19" s="28"/>
-      <c r="X19" s="28"/>
-      <c r="AF19" s="28"/>
-    </row>
-    <row r="20" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="T20" s="28"/>
+      <c r="AE19" s="28"/>
+    </row>
+    <row r="20" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="V20" s="28"/>
       <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="AF20" s="28"/>
-    </row>
-    <row r="21" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="T21" s="28"/>
+      <c r="AE20" s="28"/>
+    </row>
+    <row r="21" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="V21" s="28"/>
       <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="AF21" s="28"/>
-    </row>
-    <row r="22" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E22" s="28"/>
-      <c r="P22" s="28"/>
-      <c r="T22" s="28"/>
+      <c r="AE21" s="28"/>
+    </row>
+    <row r="22" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="V22" s="28"/>
       <c r="W22" s="28"/>
-      <c r="X22" s="28"/>
-      <c r="AF22" s="28"/>
-    </row>
-    <row r="23" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E23" s="28"/>
-      <c r="P23" s="28"/>
-      <c r="T23" s="28"/>
+      <c r="AE22" s="28"/>
+    </row>
+    <row r="23" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="S23" s="28"/>
+      <c r="V23" s="28"/>
       <c r="W23" s="28"/>
-      <c r="X23" s="28"/>
-      <c r="AF23" s="28"/>
-    </row>
-    <row r="24" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E24" s="28"/>
-      <c r="P24" s="28"/>
-      <c r="T24" s="28"/>
+      <c r="AE23" s="28"/>
+    </row>
+    <row r="24" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="V24" s="28"/>
       <c r="W24" s="28"/>
-      <c r="X24" s="28"/>
-      <c r="AF24" s="28"/>
-    </row>
-    <row r="25" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="T25" s="28"/>
+      <c r="AE24" s="28"/>
+    </row>
+    <row r="25" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="V25" s="28"/>
       <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="AF25" s="28"/>
-    </row>
-    <row r="26" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="T26" s="28"/>
+      <c r="AE25" s="28"/>
+    </row>
+    <row r="26" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="V26" s="28"/>
       <c r="W26" s="28"/>
-      <c r="X26" s="28"/>
-      <c r="AF26" s="28"/>
-    </row>
-    <row r="27" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="T27" s="28"/>
+      <c r="AE26" s="28"/>
+    </row>
+    <row r="27" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="V27" s="28"/>
       <c r="W27" s="28"/>
-      <c r="X27" s="28"/>
-      <c r="AF27" s="28"/>
-    </row>
-    <row r="28" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="T28" s="28"/>
+      <c r="AE27" s="28"/>
+    </row>
+    <row r="28" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="S28" s="28"/>
+      <c r="V28" s="28"/>
       <c r="W28" s="28"/>
-      <c r="X28" s="28"/>
-      <c r="AF28" s="28"/>
-    </row>
-    <row r="29" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E29" s="28"/>
-      <c r="P29" s="28"/>
-      <c r="T29" s="28"/>
+      <c r="AE28" s="28"/>
+    </row>
+    <row r="29" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="V29" s="28"/>
       <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="AF29" s="28"/>
-    </row>
-    <row r="30" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E30" s="28"/>
-      <c r="P30" s="28"/>
-      <c r="T30" s="28"/>
+      <c r="AE29" s="28"/>
+    </row>
+    <row r="30" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="V30" s="28"/>
       <c r="W30" s="28"/>
-      <c r="X30" s="28"/>
-      <c r="AF30" s="28"/>
-    </row>
-    <row r="31" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E31" s="28"/>
-      <c r="P31" s="28"/>
-      <c r="T31" s="28"/>
+      <c r="AE30" s="28"/>
+    </row>
+    <row r="31" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="V31" s="28"/>
       <c r="W31" s="28"/>
-      <c r="X31" s="28"/>
-      <c r="AF31" s="28"/>
-    </row>
-    <row r="32" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E32" s="28"/>
-      <c r="P32" s="28"/>
-      <c r="T32" s="28"/>
+      <c r="AE31" s="28"/>
+    </row>
+    <row r="32" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="V32" s="28"/>
       <c r="W32" s="28"/>
-      <c r="X32" s="28"/>
-      <c r="AF32" s="28"/>
-    </row>
-    <row r="33" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="T33" s="28"/>
+      <c r="AE32" s="28"/>
+    </row>
+    <row r="33" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="V33" s="28"/>
       <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
-      <c r="AF33" s="28"/>
-    </row>
-    <row r="34" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E34" s="28"/>
-      <c r="P34" s="28"/>
-      <c r="T34" s="28"/>
+      <c r="AE33" s="28"/>
+    </row>
+    <row r="34" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="V34" s="28"/>
       <c r="W34" s="28"/>
-      <c r="X34" s="28"/>
-      <c r="AF34" s="28"/>
-    </row>
-    <row r="35" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E35" s="28"/>
-      <c r="P35" s="28"/>
-      <c r="T35" s="28"/>
+      <c r="AE34" s="28"/>
+    </row>
+    <row r="35" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="V35" s="28"/>
       <c r="W35" s="28"/>
-      <c r="X35" s="28"/>
-      <c r="AF35" s="28"/>
-    </row>
-    <row r="36" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="T36" s="28"/>
+      <c r="AE35" s="28"/>
+    </row>
+    <row r="36" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="V36" s="28"/>
       <c r="W36" s="28"/>
-      <c r="X36" s="28"/>
-      <c r="AF36" s="28"/>
-    </row>
-    <row r="37" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E37" s="28"/>
-      <c r="P37" s="28"/>
-      <c r="T37" s="28"/>
+      <c r="AE36" s="28"/>
+    </row>
+    <row r="37" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="S37" s="28"/>
+      <c r="V37" s="28"/>
       <c r="W37" s="28"/>
-      <c r="X37" s="28"/>
-      <c r="AF37" s="28"/>
-    </row>
-    <row r="38" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E38" s="28"/>
-      <c r="P38" s="28"/>
-      <c r="T38" s="28"/>
+      <c r="AE37" s="28"/>
+    </row>
+    <row r="38" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="S38" s="28"/>
+      <c r="V38" s="28"/>
       <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
-      <c r="AF38" s="28"/>
-    </row>
-    <row r="39" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E39" s="28"/>
-      <c r="P39" s="28"/>
-      <c r="T39" s="28"/>
+      <c r="AE38" s="28"/>
+    </row>
+    <row r="39" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="V39" s="28"/>
       <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="AF39" s="28"/>
-    </row>
-    <row r="40" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="T40" s="28"/>
+      <c r="AE39" s="28"/>
+    </row>
+    <row r="40" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="V40" s="28"/>
       <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="AF40" s="28"/>
-    </row>
-    <row r="41" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E41" s="28"/>
-      <c r="P41" s="28"/>
-      <c r="T41" s="28"/>
+      <c r="AE40" s="28"/>
+    </row>
+    <row r="41" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="S41" s="28"/>
+      <c r="V41" s="28"/>
       <c r="W41" s="28"/>
-      <c r="X41" s="28"/>
-      <c r="AF41" s="28"/>
-    </row>
-    <row r="42" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E42" s="28"/>
-      <c r="P42" s="28"/>
-      <c r="T42" s="28"/>
+      <c r="AE41" s="28"/>
+    </row>
+    <row r="42" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="V42" s="28"/>
       <c r="W42" s="28"/>
-      <c r="X42" s="28"/>
-      <c r="AF42" s="28"/>
-    </row>
-    <row r="43" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E43" s="28"/>
-      <c r="P43" s="28"/>
-      <c r="T43" s="28"/>
+      <c r="AE42" s="28"/>
+    </row>
+    <row r="43" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D43" s="28"/>
+      <c r="O43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="V43" s="28"/>
       <c r="W43" s="28"/>
-      <c r="X43" s="28"/>
-      <c r="AF43" s="28"/>
-    </row>
-    <row r="44" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E44" s="28"/>
-      <c r="P44" s="28"/>
-      <c r="T44" s="28"/>
+      <c r="AE43" s="28"/>
+    </row>
+    <row r="44" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="V44" s="28"/>
       <c r="W44" s="28"/>
-      <c r="X44" s="28"/>
-      <c r="AF44" s="28"/>
-    </row>
-    <row r="45" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E45" s="28"/>
-      <c r="P45" s="28"/>
-      <c r="T45" s="28"/>
+      <c r="AE44" s="28"/>
+    </row>
+    <row r="45" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="V45" s="28"/>
       <c r="W45" s="28"/>
-      <c r="X45" s="28"/>
-      <c r="AF45" s="28"/>
-    </row>
-    <row r="46" spans="5:32" x14ac:dyDescent="0.2">
-      <c r="E46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="T46" s="28"/>
+      <c r="AE45" s="28"/>
+    </row>
+    <row r="46" spans="4:31" x14ac:dyDescent="0.2">
+      <c r="D46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="S46" s="28"/>
+      <c r="V46" s="28"/>
       <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
-      <c r="AF46" s="28"/>
+      <c r="AE46" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="28" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB46 AJ3:AJ46" xr:uid="{18B55665-E7A6-43AF-9477-C1A0427DF4D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA10:AA46 AJ3:AJ9 AI10:AI46 AB3:AB9" xr:uid="{18B55665-E7A6-43AF-9477-C1A0427DF4D8}">
       <formula1>"single,paired"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6236,31 +6249,31 @@
           <x14:formula1>
             <xm:f>'Library and Platform Names'!$C$87:$C$107</xm:f>
           </x14:formula1>
-          <xm:sqref>X3:X46</xm:sqref>
+          <xm:sqref>W10:W46 X3:X9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D9348EC4-84CA-4ADF-8D4B-09EBD483E08D}">
           <x14:formula1>
             <xm:f>'Library and Platform Names'!$A$3:$A$37</xm:f>
           </x14:formula1>
-          <xm:sqref>Y3:Y46 AG3:AG46</xm:sqref>
+          <xm:sqref>X10:X46 AG3:AG9 AF10:AF46 Y3:Y9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{874EA618-F782-47F4-8D31-92C5AE0CE9DB}">
           <x14:formula1>
             <xm:f>'Library and Platform Names'!$A$40:$A$48</xm:f>
           </x14:formula1>
-          <xm:sqref>Z3:Z46 AH3:AH46</xm:sqref>
+          <xm:sqref>Y10:Y46 AH3:AH9 AG10:AG46 Z3:Z9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C77280A-9F37-459A-9D85-07464EB08E8F}">
           <x14:formula1>
             <xm:f>'Library and Platform Names'!$A$51:$A$83</xm:f>
           </x14:formula1>
-          <xm:sqref>AA3:AA46 AI3:AI46</xm:sqref>
+          <xm:sqref>Z10:Z46 AI3:AI9 AH10:AH46 AA3:AA9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46D7318A-3F29-4C22-8B3C-B0561D2959F7}">
           <x14:formula1>
             <xm:f>'Library and Platform Names'!$J$87:$J$89</xm:f>
           </x14:formula1>
-          <xm:sqref>AF3:AF46</xm:sqref>
+          <xm:sqref>AE10:AE46 AF3:AF9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10021,15 +10034,48 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
@@ -10042,48 +10088,15 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
made fake fastq files and real fastq paths for test submission
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9195130-6292-BA40-A463-EE2266FC9555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EB7937-55A1-A945-950C-036F3AA59A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2876,7 +2876,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="423">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4081,36 +4081,6 @@
     <t>MPXV_TX0001</t>
   </si>
   <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/2022-053-7721_S6_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/2022-053-7721_S6_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/groups-pure/Projects/scbs_mpob/data/mpx_filtered/LIY15306A2_2022_054_3005007722.R_1.mpx.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/groups-pure/Projects/scbs_mpob/data/mpx_filtered/LIY15306A2_2022_054_3005007722.R_2.mpx.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-028-7666_S3_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-028-7666_S3_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-029-7670_S4_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-029-7670_S4_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-034-7690_S9_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-034-7690_S9_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
     <t>FL0015</t>
   </si>
   <si>
@@ -4163,6 +4133,18 @@
   </si>
   <si>
     <t>fasta_name</t>
+  </si>
+  <si>
+    <t>$PWD/assets/sample_fastqs/sample1_R1.fastq</t>
+  </si>
+  <si>
+    <t>$PWD/assets/sample_fastqs/sample3_R1.fastq</t>
+  </si>
+  <si>
+    <t>$PWD/assets/sample_fastqs/sample4_R1.fastq</t>
+  </si>
+  <si>
+    <t>$PWD/assets/sample_fastqs/sample1_R2.fastq</t>
   </si>
 </sst>
 </file>
@@ -4172,7 +4154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4393,6 +4375,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="42">
@@ -4814,7 +4803,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4862,6 +4851,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5296,8 +5286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB79B10-5F4B-4CF2-A235-6BD3FDFF8F8F}">
   <dimension ref="A1:AL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AG12" sqref="AG12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5338,31 +5328,31 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>12</v>
@@ -5454,7 +5444,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
         <v>372</v>
@@ -5469,7 +5459,7 @@
         <v>377</v>
       </c>
       <c r="G3" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H3" t="s">
         <v>386</v>
@@ -5515,16 +5505,16 @@
         <v>61</v>
       </c>
       <c r="AD3" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="AE3" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="AF3" s="28"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s">
         <v>373</v>
@@ -5539,7 +5529,7 @@
         <v>378</v>
       </c>
       <c r="G4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H4" t="s">
         <v>386</v>
@@ -5581,17 +5571,17 @@
       <c r="AB4" t="s">
         <v>61</v>
       </c>
-      <c r="AD4" t="s">
-        <v>403</v>
+      <c r="AD4" s="37" t="s">
+        <v>419</v>
       </c>
       <c r="AE4" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="AF4" s="28"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
         <v>374</v>
@@ -5606,7 +5596,7 @@
         <v>379</v>
       </c>
       <c r="G5" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
         <v>386</v>
@@ -5649,16 +5639,16 @@
         <v>61</v>
       </c>
       <c r="AD5" t="s">
-        <v>405</v>
+        <v>420</v>
       </c>
       <c r="AE5" t="s">
-        <v>406</v>
+        <v>422</v>
       </c>
       <c r="AF5" s="28"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B6" t="s">
         <v>375</v>
@@ -5673,7 +5663,7 @@
         <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H6" t="s">
         <v>386</v>
@@ -5719,16 +5709,16 @@
         <v>61</v>
       </c>
       <c r="AD6" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="AE6" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
       <c r="AF6" s="28"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B7" t="s">
         <v>376</v>
@@ -5743,7 +5733,7 @@
         <v>381</v>
       </c>
       <c r="G7" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H7" t="s">
         <v>386</v>
@@ -5789,19 +5779,19 @@
         <v>61</v>
       </c>
       <c r="AD7" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE7" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="AF7" s="28"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="B8" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C8" t="s">
         <v>381</v>
@@ -5813,7 +5803,7 @@
         <v>381</v>
       </c>
       <c r="G8" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H8" t="s">
         <v>386</v>
@@ -5859,19 +5849,19 @@
         <v>61</v>
       </c>
       <c r="AD8" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE8" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="AF8" s="28"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="C9" t="s">
         <v>381</v>
@@ -5883,7 +5873,7 @@
         <v>381</v>
       </c>
       <c r="G9" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H9" t="s">
         <v>386</v>
@@ -5929,10 +5919,10 @@
         <v>61</v>
       </c>
       <c r="AD9" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE9" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="AF9" s="28"/>
     </row>
@@ -10034,12 +10024,51 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -10052,51 +10081,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added test fastqs to assets
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/MPXV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9195130-6292-BA40-A463-EE2266FC9555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD70963-2EE7-FD44-A611-6B07DD2FF319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -433,7 +433,7 @@
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -442,7 +442,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2876,7 +2876,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="421">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4081,36 +4081,6 @@
     <t>MPXV_TX0001</t>
   </si>
   <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/2022-053-7721_S6_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/2022-053-7721_S6_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/groups-pure/Projects/scbs_mpob/data/mpx_filtered/LIY15306A2_2022_054_3005007722.R_1.mpx.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/groups-pure/Projects/scbs_mpob/data/mpx_filtered/LIY15306A2_2022_054_3005007722.R_2.mpx.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-028-7666_S3_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-028-7666_S3_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-029-7670_S4_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-029-7670_S4_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-034-7690_S9_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220611_M03083_0092_000000000-J88KR/Alignment_1/20220613_231902/Fastq/2022-034-7690_S9_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
     <t>FL0015</t>
   </si>
   <si>
@@ -4163,6 +4133,12 @@
   </si>
   <si>
     <t>fasta_name</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/SRR27947460sub_1.fastq</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/SRR27947460sub_2.fastq</t>
   </si>
 </sst>
 </file>
@@ -4172,7 +4148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4389,6 +4365,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
@@ -5296,8 +5279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB79B10-5F4B-4CF2-A235-6BD3FDFF8F8F}">
   <dimension ref="A1:AL46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4:AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5338,31 +5321,31 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>12</v>
@@ -5454,7 +5437,7 @@
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
         <v>372</v>
@@ -5469,7 +5452,7 @@
         <v>377</v>
       </c>
       <c r="G3" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H3" t="s">
         <v>386</v>
@@ -5515,16 +5498,16 @@
         <v>61</v>
       </c>
       <c r="AD3" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="AE3" t="s">
-        <v>402</v>
+        <v>420</v>
       </c>
       <c r="AF3" s="28"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s">
         <v>373</v>
@@ -5539,7 +5522,7 @@
         <v>378</v>
       </c>
       <c r="G4" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H4" t="s">
         <v>386</v>
@@ -5582,16 +5565,16 @@
         <v>61</v>
       </c>
       <c r="AD4" t="s">
-        <v>403</v>
+        <v>419</v>
       </c>
       <c r="AE4" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="AF4" s="28"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
         <v>374</v>
@@ -5606,7 +5589,7 @@
         <v>379</v>
       </c>
       <c r="G5" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
         <v>386</v>
@@ -5649,16 +5632,16 @@
         <v>61</v>
       </c>
       <c r="AD5" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="AE5" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
       <c r="AF5" s="28"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B6" t="s">
         <v>375</v>
@@ -5673,7 +5656,7 @@
         <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H6" t="s">
         <v>386</v>
@@ -5719,16 +5702,16 @@
         <v>61</v>
       </c>
       <c r="AD6" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="AE6" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="AF6" s="28"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B7" t="s">
         <v>376</v>
@@ -5743,7 +5726,7 @@
         <v>381</v>
       </c>
       <c r="G7" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H7" t="s">
         <v>386</v>
@@ -5789,19 +5772,19 @@
         <v>61</v>
       </c>
       <c r="AD7" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE7" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="AF7" s="28"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="B8" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C8" t="s">
         <v>381</v>
@@ -5813,7 +5796,7 @@
         <v>381</v>
       </c>
       <c r="G8" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H8" t="s">
         <v>386</v>
@@ -5859,19 +5842,19 @@
         <v>61</v>
       </c>
       <c r="AD8" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE8" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="AF8" s="28"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B9" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="C9" t="s">
         <v>381</v>
@@ -5883,7 +5866,7 @@
         <v>381</v>
       </c>
       <c r="G9" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="H9" t="s">
         <v>386</v>
@@ -5929,10 +5912,10 @@
         <v>61</v>
       </c>
       <c r="AD9" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="AE9" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="AF9" s="28"/>
     </row>
@@ -10034,12 +10017,51 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -10052,51 +10074,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>